<commit_message>
Ajout de la librairie JSISO
</commit_message>
<xml_diff>
--- a/Doc/B65_-_Hiver_2017_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
+++ b/Doc/B65_-_Hiver_2017_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
@@ -2643,7 +2643,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2962,7 +2961,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3069,7 +3067,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3382,7 +3379,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3489,7 +3485,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3817,7 +3812,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3924,7 +3918,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4281,7 +4274,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>

</xml_diff>